<commit_message>
Updated logic with list of jobs
</commit_message>
<xml_diff>
--- a/Development/Smoker Profile Logic.xlsx
+++ b/Development/Smoker Profile Logic.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19017"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F9CAF11-B334-4FC9-97FC-7C4DBDDEB518}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrien/OneDrive - Thrive Tribe/Lify App/App/Development/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Logic" sheetId="1" r:id="rId1"/>
+    <sheet name="Jobs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171026"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>Profiles</t>
   </si>
@@ -111,13 +116,40 @@
   </si>
   <si>
     <t>Is smoking concerning you about the future?</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Job type</t>
+  </si>
+  <si>
+    <t>Creative and art professional</t>
+  </si>
+  <si>
+    <t>Professional and Managers</t>
+  </si>
+  <si>
+    <t>Manual Work</t>
+  </si>
+  <si>
+    <t>User profile</t>
+  </si>
+  <si>
+    <t>Note: Screen to be visual with cards</t>
+  </si>
+  <si>
+    <t>Unemployed and retired</t>
+  </si>
+  <si>
+    <t>Students/youngster (&lt;30)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,15 +176,45 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -216,16 +278,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -233,12 +292,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -248,12 +301,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,290 +646,290 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A13" sqref="A13:A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="B2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="B3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="B4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="16"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="6" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="15" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="13" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="16">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="12">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="16">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="12">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="12">
         <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="16">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="12">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="16">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="12">
         <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="16">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="12">
         <v>6</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="16">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="12">
         <v>7</v>
       </c>
       <c r="B22" t="s">
@@ -861,34 +937,126 @@
       </c>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="14.25" customHeight="1">
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D50837-8A87-474D-8EE6-9B758ECB0C1B}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="24"/>
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="13"/>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="13"/>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>